<commit_message>
Lol actually everything is fine and there wasn't a problem with the merge geoprocessing and I finished 07.2.R
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/05b_edited1_conflicting-multiple-treatments_fixed.xlsx
+++ b/data/data-wrangling-intermediate/05b_edited1_conflicting-multiple-treatments_fixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/04_LDC-LTDL/LDC-LTDL_v02/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:b_{6ECEE7FE-43EF-4F3B-BB6C-8A8CD8D6B5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:b_{6ECEE7FE-43EF-4F3B-BB6C-8A8CD8D6B5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D0B5DA4-99F0-4F7B-A79B-1CCF9B95CCF3}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13944" xr2:uid="{14C02F12-2078-444B-9311-36E6A60FEF3D}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13944" activeTab="1" xr2:uid="{14C02F12-2078-444B-9311-36E6A60FEF3D}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="2" r:id="rId1"/>
@@ -791,7 +791,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>(Same as 05.7a.xlsx from  Proejct v01)</a:t>
+            <a:t>(Same as 05.7a.xlsx from  Project v01)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1189,7 +1189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807A1632-160F-425F-97D4-B9B9B457B6D7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -1202,9 +1204,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823587FF-1FD9-42E0-9D52-1D7FB3DBCCC8}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>